<commit_message>
Add Manual Test Script
</commit_message>
<xml_diff>
--- a/CompetitionTaskProjectMars/ManualTestScript/Competition task test cases.xlsx
+++ b/CompetitionTaskProjectMars/ManualTestScript/Competition task test cases.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="152">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -394,6 +395,87 @@
   </si>
   <si>
     <t>Certification record is deleted</t>
+  </si>
+  <si>
+    <t>TS_007</t>
+  </si>
+  <si>
+    <t>Validate user trying to update profile about me components</t>
+  </si>
+  <si>
+    <t>TC_016 Verify user able to update about me components in profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. click on the name </t>
+  </si>
+  <si>
+    <t>3. Edit the record by adding first name and last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Cick in the location and try to edit location </t>
+  </si>
+  <si>
+    <t>5. Click on the Avaliability edit pencil and change avaliability to full time or part time</t>
+  </si>
+  <si>
+    <t>7. click on the Earn Target edit pencil icon and change it</t>
+  </si>
+  <si>
+    <t>Samma Sachethanie</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>Part time</t>
+  </si>
+  <si>
+    <t>less than 30 hours a week</t>
+  </si>
+  <si>
+    <t>less tha $500 per month</t>
+  </si>
+  <si>
+    <t>1. click on the profile photo and add a photo</t>
+  </si>
+  <si>
+    <t>User should be able to add profile photo</t>
+  </si>
+  <si>
+    <t>User should be able to edit first name and last name</t>
+  </si>
+  <si>
+    <t>User should be able to edit location</t>
+  </si>
+  <si>
+    <t>User should be able to edit availability</t>
+  </si>
+  <si>
+    <t>User should be able to edit Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. click on the hours edit pencil icon and change it </t>
+  </si>
+  <si>
+    <t>User should be able to edit Earn Target</t>
+  </si>
+  <si>
+    <t>User cannot be able to add profile photo</t>
+  </si>
+  <si>
+    <t>User can be able to edit first name and last name</t>
+  </si>
+  <si>
+    <t>User cannot be able to edit location</t>
+  </si>
+  <si>
+    <t>User can be able to edit availability</t>
+  </si>
+  <si>
+    <t>User can be able to edit Hours</t>
+  </si>
+  <si>
+    <t>User can be able to edit Earn Target</t>
   </si>
 </sst>
 </file>
@@ -456,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -503,12 +585,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,25 +681,92 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -852,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67:I71"/>
+    <sheetView topLeftCell="D39" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,16 +1097,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -916,214 +1115,214 @@
       <c r="F2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="18"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="23" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="25" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="18"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="18"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="18"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="22" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="22"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="22"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="22"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="10" t="s">
         <v>86</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="22"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="10" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="22"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="22"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="10" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="11">
         <v>2018</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="22"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="22"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="22" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1132,68 +1331,68 @@
       <c r="F16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="18"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="18"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="18"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="18" t="s">
+      <c r="A20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -1202,77 +1401,77 @@
       <c r="F20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="18"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="22"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="18"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="22"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="18"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="22"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="8"/>
       <c r="F24" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="18"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="13" t="s">
         <v>96</v>
       </c>
@@ -1292,16 +1491,16 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -1310,81 +1509,81 @@
       <c r="F26" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="18"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="18"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="18"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="8"/>
       <c r="F30" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="18"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="18" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E31" s="8" t="s">
@@ -1393,156 +1592,156 @@
       <c r="F31" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="18"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
       <c r="E33" s="8" t="s">
         <v>81</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="18"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="20"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="18"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="18"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="20"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="8"/>
       <c r="F35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="18"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="20"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F36" s="8"/>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I36" s="18" t="s">
+      <c r="I36" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="18"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="18"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="20"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="18"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="20"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="18"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="18"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="18"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E41" s="8" t="s">
@@ -1551,105 +1750,105 @@
       <c r="F41" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G41" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="I41" s="27" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="19"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="22"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="24"/>
       <c r="E42" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="17"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="19"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="22"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="24"/>
       <c r="E43" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="17"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="22"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="24"/>
       <c r="E44" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F44" s="8"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="17"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="19"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="22"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="24"/>
       <c r="E45" s="10" t="s">
         <v>87</v>
       </c>
       <c r="F45" s="8"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="22"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="24"/>
       <c r="E46" s="10" t="s">
         <v>88</v>
       </c>
       <c r="F46" s="8"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="17"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="22"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="24"/>
       <c r="E47" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F47" s="8"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="17"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="19"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="22" t="s">
+      <c r="A48" s="22"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="8" t="s">
@@ -1658,64 +1857,64 @@
       <c r="F48" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G48" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H48" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="I48" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G49" s="18"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="18"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="19"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
       <c r="E50" s="10" t="s">
         <v>89</v>
       </c>
       <c r="F50" s="8"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="18"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="19"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
       <c r="E51" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F51" s="8"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="18"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="20"/>
     </row>
     <row r="52" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="19"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="22" t="s">
+      <c r="A52" s="22"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="22" t="s">
+      <c r="D52" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="8" t="s">
@@ -1724,60 +1923,60 @@
       <c r="F52" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G52" s="18" t="s">
+      <c r="G52" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H52" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I52" s="18" t="s">
+      <c r="I52" s="20" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="19"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
       <c r="E53" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G53" s="18"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="18"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="20"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="19"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
       <c r="E54" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G54" s="18"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="18"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="20"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="19"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="16"/>
-      <c r="I55" s="18"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="20"/>
     </row>
     <row r="56" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="19"/>
-      <c r="B56" s="20"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="21"/>
       <c r="C56" s="13" t="s">
         <v>106</v>
       </c>
@@ -1797,16 +1996,16 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E57" s="8" t="s">
@@ -1815,219 +2014,219 @@
       <c r="F57" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G57" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="H57" s="16" t="s">
+      <c r="H57" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I57" s="18" t="s">
+      <c r="I57" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="19"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="22"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="24"/>
       <c r="E58" s="8" t="s">
         <v>101</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G58" s="18"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="18"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="20"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="19"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="22"/>
+      <c r="A59" s="22"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="24"/>
       <c r="E59" s="8" t="s">
         <v>102</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G59" s="18"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="18"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="20"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="19"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="22"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="24"/>
       <c r="E60" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F60" s="8"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="18"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="20"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="19"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="18"/>
+      <c r="A61" s="22"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="20"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="18"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="20"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="19"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="18" t="s">
+      <c r="A62" s="22"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D62" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>84</v>
       </c>
       <c r="F62" s="8"/>
-      <c r="G62" s="18" t="s">
+      <c r="G62" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="H62" s="16" t="s">
+      <c r="H62" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I62" s="20" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="19"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="22"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="24"/>
       <c r="E63" s="8" t="s">
         <v>101</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G63" s="18"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="18"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="20"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" s="19"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="22"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="24"/>
       <c r="E64" s="8" t="s">
         <v>103</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G64" s="18"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="18"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="20"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" s="19"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="22"/>
+      <c r="A65" s="22"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="24"/>
       <c r="E65" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G65" s="18"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="18"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="20"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66" s="19"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="22"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="18"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="20"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="C67" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F67" s="8"/>
-      <c r="G67" s="18" t="s">
+      <c r="G67" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="H67" s="16" t="s">
+      <c r="H67" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I67" s="18" t="s">
+      <c r="I67" s="20" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A68" s="19"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="18"/>
+      <c r="A68" s="22"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="20"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="16"/>
-      <c r="I68" s="18"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="20"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69" s="19"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="18"/>
+      <c r="A69" s="22"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="20"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="18"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="20"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70" s="19"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="18"/>
+      <c r="A70" s="22"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="18"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="20"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" s="19"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="18"/>
+      <c r="A71" s="22"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="18"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="20"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
@@ -2039,20 +2238,54 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="I7:I15"/>
-    <mergeCell ref="H7:H15"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="H36:H40"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="H57:H61"/>
+    <mergeCell ref="H62:H66"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="C67:C71"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="H67:H71"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="I67:I71"/>
+    <mergeCell ref="B57:B66"/>
+    <mergeCell ref="A57:A66"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="A41:A56"/>
+    <mergeCell ref="B41:B56"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="D31:D35"/>
     <mergeCell ref="G31:G35"/>
     <mergeCell ref="I31:I35"/>
     <mergeCell ref="B26:B35"/>
@@ -2069,54 +2302,20 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="G2:G6"/>
     <mergeCell ref="G20:G24"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="A41:A56"/>
-    <mergeCell ref="B41:B56"/>
-    <mergeCell ref="D41:D47"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="C67:C71"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="H67:H71"/>
-    <mergeCell ref="G67:G71"/>
-    <mergeCell ref="I67:I71"/>
-    <mergeCell ref="B57:B66"/>
-    <mergeCell ref="A57:A66"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="G62:G66"/>
-    <mergeCell ref="I62:I66"/>
-    <mergeCell ref="H52:H55"/>
-    <mergeCell ref="H57:H61"/>
-    <mergeCell ref="H62:H66"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="H31:H35"/>
-    <mergeCell ref="H36:H40"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="I7:I15"/>
+    <mergeCell ref="H7:H15"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="H20:H24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -2124,4 +2323,1410 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.36328125" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+    <col min="6" max="6" width="34.08984375" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" customWidth="1"/>
+    <col min="9" max="9" width="28.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="34"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="34"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="34"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="34"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="34"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="34"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="34"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="34"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="34"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="34"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
+    </row>
+    <row r="14" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="34"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="19">
+        <v>2018</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="34"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="34"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="34"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="34"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="34"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="34"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="34"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="34"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="34"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="34"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="34"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="34"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="34"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="34"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="34"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="34"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="34"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="34"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="20"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="34"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="34"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="34"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="34"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="34"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="34"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H41" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="34"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="34"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="34"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="20"/>
+    </row>
+    <row r="45" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="34"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="20"/>
+    </row>
+    <row r="46" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="34"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="34"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="34"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="34"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" s="35"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="20"/>
+    </row>
+    <row r="50" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="34"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="20"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="34"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="20"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="34"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H52" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I52" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="34"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G53" s="20"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="20"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="34"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G54" s="20"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="20"/>
+    </row>
+    <row r="55" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="34"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="20"/>
+    </row>
+    <row r="56" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="34"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I57" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="34"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G58" s="20"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="34"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G59" s="20"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="34"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="34"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="20"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="34"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="G62" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I62" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="34"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G63" s="20"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="20"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="34"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G64" s="20"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="20"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="34"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G65" s="20"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="20"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="34"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="20"/>
+    </row>
+    <row r="67" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F67" s="8"/>
+      <c r="G67" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H67" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="34"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="20"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="34"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="20"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="34"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="20"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="34"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="20"/>
+    </row>
+    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" s="8"/>
+      <c r="G72" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H72" s="16"/>
+      <c r="I72" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="45"/>
+      <c r="B73" s="41"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F73" s="8"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="12"/>
+    </row>
+    <row r="74" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A74" s="45"/>
+      <c r="B74" s="41"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="H74" s="43"/>
+      <c r="I74" s="39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="45"/>
+      <c r="B75" s="41"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H75" s="43"/>
+      <c r="I75" s="39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="45"/>
+      <c r="B76" s="41"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="H76" s="43"/>
+      <c r="I76" s="39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="45"/>
+      <c r="B77" s="41"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="41"/>
+      <c r="E77" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="H77" s="43"/>
+      <c r="I77" s="39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="46"/>
+      <c r="B78" s="42"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="H78" s="43"/>
+      <c r="I78" s="39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="82">
+    <mergeCell ref="C72:C78"/>
+    <mergeCell ref="D72:D78"/>
+    <mergeCell ref="A72:A78"/>
+    <mergeCell ref="B72:B78"/>
+    <mergeCell ref="I67:I71"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="C67:C71"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="H67:H71"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="H62:H66"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="A57:A66"/>
+    <mergeCell ref="B57:B66"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="H57:H61"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="A41:A56"/>
+    <mergeCell ref="B41:B56"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="H36:H40"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="D7:D15"/>
+    <mergeCell ref="G7:G15"/>
+    <mergeCell ref="H7:H15"/>
+    <mergeCell ref="I7:I15"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="H2:H6"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>